<commit_message>
Changes made for class and asynchronous
</commit_message>
<xml_diff>
--- a/runManager/RunSheet_Date.xlsx
+++ b/runManager/RunSheet_Date.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="48">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -656,41 +656,71 @@
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -710,49 +740,85 @@
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -772,17 +838,29 @@
       <c r="A25" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">

</xml_diff>